<commit_message>
Adição dos slides da apresentação
</commit_message>
<xml_diff>
--- a/Documentação/BackLog - Projeto Individual.xlsx
+++ b/Documentação/BackLog - Projeto Individual.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\VSCode\SPTECH\PI\Sophrosyne\Documentação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SPTech\Pesquisa e Inovação\Sophrosyne\Documentação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5666A72C-1187-494B-BCCD-4978E500211A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F0A1C62-EDBF-48A8-94A6-F628C7E665BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{462F1E4E-284A-401C-A6EC-788D4F3EAE0D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{462F1E4E-284A-401C-A6EC-788D4F3EAE0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="66">
   <si>
     <t>Requisito</t>
   </si>
@@ -104,12 +104,6 @@
     <t>Finalizado</t>
   </si>
   <si>
-    <t>Em andamento</t>
-  </si>
-  <si>
-    <t>Pendente</t>
-  </si>
-  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -155,9 +149,6 @@
     <t>Diagrama de solução</t>
   </si>
   <si>
-    <t>Gráfico de burndown</t>
-  </si>
-  <si>
     <t>Preparação do PPT</t>
   </si>
   <si>
@@ -225,9 +216,6 @@
   </si>
   <si>
     <t>Desenvolver o diagram de solução do projeto</t>
-  </si>
-  <si>
-    <t>Adicionar o grafico de burndown do projeto</t>
   </si>
   <si>
     <t>Desenvolver a apresentação do projeto</t>
@@ -994,8 +982,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1113EAA2-1D9B-4E88-BAC2-D37E62E498FA}" name="Tabela3" displayName="Tabela3" ref="B2:J26" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
-  <autoFilter ref="B2:J26" xr:uid="{1113EAA2-1D9B-4E88-BAC2-D37E62E498FA}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{1113EAA2-1D9B-4E88-BAC2-D37E62E498FA}" name="Tabela3" displayName="Tabela3" ref="B2:J25" totalsRowShown="0" headerRowDxfId="19" dataDxfId="17" headerRowBorderDxfId="18" tableBorderDxfId="16" totalsRowBorderDxfId="15">
+  <autoFilter ref="B2:J25" xr:uid="{1113EAA2-1D9B-4E88-BAC2-D37E62E498FA}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B3:J19">
     <sortCondition ref="H2:H19"/>
   </sortState>
@@ -1331,10 +1319,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F914F649-CA56-42D2-8C7C-73F90C16BA67}">
-  <dimension ref="B2:M26"/>
+  <dimension ref="B2:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20:I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1384,7 +1372,7 @@
         <v>20</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>14</v>
@@ -1410,10 +1398,10 @@
     </row>
     <row r="4" spans="2:13" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B4" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>14</v>
@@ -1442,7 +1430,7 @@
         <v>10</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>14</v>
@@ -1466,15 +1454,15 @@
         <v>9</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D6" s="5" t="s">
         <v>14</v>
@@ -1500,10 +1488,10 @@
     </row>
     <row r="7" spans="2:13" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>14</v>
@@ -1532,7 +1520,7 @@
         <v>11</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="D8" s="5" t="s">
         <v>14</v>
@@ -1558,10 +1546,10 @@
     </row>
     <row r="9" spans="2:13" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D9" s="5" t="s">
         <v>14</v>
@@ -1587,10 +1575,10 @@
     </row>
     <row r="10" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>14</v>
@@ -1619,7 +1607,7 @@
         <v>13</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>14</v>
@@ -1645,10 +1633,10 @@
     </row>
     <row r="12" spans="2:13" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B12" s="4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D12" s="5" t="s">
         <v>14</v>
@@ -1677,7 +1665,7 @@
         <v>12</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>14</v>
@@ -1703,10 +1691,10 @@
     </row>
     <row r="14" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B14" s="4" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>14</v>
@@ -1732,13 +1720,13 @@
     </row>
     <row r="15" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B15" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E15" s="5">
         <v>13</v>
@@ -1753,7 +1741,7 @@
         <v>3</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J15" s="7" t="s">
         <v>9</v>
@@ -1761,13 +1749,13 @@
     </row>
     <row r="16" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B16" s="4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E16" s="5">
         <v>13</v>
@@ -1782,7 +1770,7 @@
         <v>3</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J16" s="7" t="s">
         <v>9</v>
@@ -1790,13 +1778,13 @@
     </row>
     <row r="17" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="E17" s="5">
         <v>13</v>
@@ -1811,7 +1799,7 @@
         <v>3</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="J17" s="7" t="s">
         <v>9</v>
@@ -1819,10 +1807,10 @@
     </row>
     <row r="18" spans="2:12" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B18" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>14</v>
@@ -1848,10 +1836,10 @@
     </row>
     <row r="19" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B19" s="12" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="D19" s="14" t="s">
         <v>14</v>
@@ -1877,10 +1865,10 @@
     </row>
     <row r="20" spans="2:12" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="D20" s="14" t="s">
         <v>14</v>
@@ -1906,10 +1894,10 @@
     </row>
     <row r="21" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D21" s="14" t="s">
         <v>14</v>
@@ -1927,7 +1915,7 @@
         <v>4</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J21" s="15" t="s">
         <v>9</v>
@@ -1936,10 +1924,10 @@
     </row>
     <row r="22" spans="2:12" ht="30.75" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>14</v>
@@ -1957,7 +1945,7 @@
         <v>4</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J22" s="7" t="s">
         <v>9</v>
@@ -1965,10 +1953,10 @@
     </row>
     <row r="23" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D23" s="14" t="s">
         <v>14</v>
@@ -1986,7 +1974,7 @@
         <v>3</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J23" s="15" t="s">
         <v>9</v>
@@ -1994,10 +1982,10 @@
     </row>
     <row r="24" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B24" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="D24" s="14" t="s">
         <v>14</v>
@@ -2009,78 +1997,49 @@
         <v>16</v>
       </c>
       <c r="G24" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H24" s="5">
         <v>4</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J24" s="15" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="25" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>64</v>
+      <c r="B25" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>61</v>
       </c>
       <c r="D25" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E25" s="5">
-        <v>5</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="G25" s="5">
+        <v>65</v>
+      </c>
+      <c r="E25" s="14">
         <v>3</v>
       </c>
-      <c r="H25" s="5">
+      <c r="F25" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="14">
+        <v>3</v>
+      </c>
+      <c r="H25" s="14">
         <v>4</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J25" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="D26" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="E26" s="14">
-        <v>3</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="G26" s="14">
-        <v>3</v>
-      </c>
-      <c r="H26" s="14">
-        <v>4</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J26" s="15" t="s">
-        <v>9</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="D3:D26">
+  <conditionalFormatting sqref="D3:D25">
     <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Desejável">
       <formula>NOT(ISERROR(SEARCH("Desejável",D3)))</formula>
     </cfRule>
@@ -2091,7 +2050,7 @@
       <formula>NOT(ISERROR(SEARCH("Essencial",D3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I26">
+  <conditionalFormatting sqref="I3:I25">
     <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Pendente">
       <formula>NOT(ISERROR(SEARCH("Pendente",I3)))</formula>
     </cfRule>
@@ -2103,10 +2062,10 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I26" xr:uid="{ED0A389E-8D43-4D26-BFC8-7ED57DB7C534}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I25" xr:uid="{ED0A389E-8D43-4D26-BFC8-7ED57DB7C534}">
       <formula1>"Finalizado,Em andamento,Pendente"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D26" xr:uid="{E0BAAABF-3205-4A4A-99A3-D31744D35852}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D25" xr:uid="{E0BAAABF-3205-4A4A-99A3-D31744D35852}">
       <formula1>"Essencial,Importante,Desejável"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>